<commit_message>
Updated with additional validation and constraint support
</commit_message>
<xml_diff>
--- a/src/test/xlsTestFiles/test-participant.xlsx
+++ b/src/test/xlsTestFiles/test-participant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Desktop/coding/xlsUploader/src/test/xlsTestFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24027896-A355-1D43-961B-7BDB7C76909C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8A2E33-7039-E84A-9446-365A1EF41D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{B474F3A5-C3F8-2345-A3DB-673EF3609AE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Participant ID</t>
   </si>
@@ -84,12 +84,18 @@
   </si>
   <si>
     <t>Johnson</t>
+  </si>
+  <si>
+    <t>Bob@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,7 +134,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +472,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,7 +481,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -491,7 +497,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -509,7 +515,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -526,7 +532,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>45718</v>
+        <v>46082</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,11 +545,17 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="2">
-        <v>45719</v>
+        <v>46082</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{2337A011-3FDD-A746-BDA1-410A0C70FF96}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>